<commit_message>
debugging build script + adding script to compare instance
</commit_message>
<xml_diff>
--- a/inst/documentation/DODO-F1000-publication/data/benchmark_summary.xlsx
+++ b/inst/documentation/DODO-F1000-publication/data/benchmark_summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\U060109.UCB-CORP\OneDrive - UCB\Documents\DODO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="41" documentId="8_{D2FFAB0A-77D5-44A4-8A08-0AEF86BFC611}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{81FB1574-7039-4FDF-9CF3-74D641A47B3E}"/>
+  <xr:revisionPtr revIDLastSave="119" documentId="8_{D2FFAB0A-77D5-44A4-8A08-0AEF86BFC611}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{098F74D7-FA06-4A43-8832-A3C86638C77A}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6490" activeTab="1" xr2:uid="{FC61BD86-EE65-4EE4-A6E1-7CC6E84CF18A}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6500" activeTab="1" xr2:uid="{FC61BD86-EE65-4EE4-A6E1-7CC6E84CF18A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -154,6 +154,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -235,7 +238,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -281,11 +284,88 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -323,13 +403,60 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -652,17 +779,17 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="A1:G14"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="38" style="12" customWidth="1"/>
-    <col min="2" max="2" width="17.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.54296875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.453125" customWidth="1"/>
     <col min="4" max="4" width="12.81640625" customWidth="1"/>
-    <col min="5" max="5" width="12.26953125" customWidth="1"/>
-    <col min="6" max="6" width="14.6328125" customWidth="1"/>
+    <col min="5" max="5" width="12.26953125" style="20" customWidth="1"/>
+    <col min="6" max="6" width="14.54296875" customWidth="1"/>
     <col min="7" max="7" width="37.26953125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -676,11 +803,11 @@
       <c r="C1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
       <c r="G1" s="2" t="s">
         <v>1</v>
       </c>
@@ -689,13 +816,13 @@
       <c r="A2" s="3"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="15" t="s">
+      <c r="F2" s="13" t="s">
         <v>4</v>
       </c>
       <c r="G2" s="4"/>
@@ -707,7 +834,7 @@
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
+      <c r="E3" s="30"/>
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
     </row>
@@ -716,16 +843,16 @@
         <v>11</v>
       </c>
       <c r="B4" s="6">
-        <v>2.9889999999999999</v>
+        <v>2989</v>
       </c>
       <c r="C4" s="6">
-        <v>2.9990000000000001</v>
+        <v>2999</v>
       </c>
       <c r="D4" s="6">
         <v>1</v>
       </c>
-      <c r="E4" s="13">
-        <v>1006</v>
+      <c r="E4" s="31">
+        <v>1.006</v>
       </c>
       <c r="F4" s="6">
         <v>2</v>
@@ -739,16 +866,16 @@
         <v>12</v>
       </c>
       <c r="B5" s="6">
-        <v>3.621</v>
+        <v>3621</v>
       </c>
       <c r="C5" s="6">
-        <v>3.15</v>
+        <v>3150</v>
       </c>
       <c r="D5" s="6">
         <v>1</v>
       </c>
-      <c r="E5" s="13">
-        <v>1145</v>
+      <c r="E5" s="31">
+        <v>1.145</v>
       </c>
       <c r="F5" s="6">
         <v>9</v>
@@ -757,21 +884,21 @@
         <v>378</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="11" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="9">
-        <v>3.944</v>
+        <v>3944</v>
       </c>
       <c r="C6" s="8">
-        <v>3.1520000000000001</v>
+        <v>3152</v>
       </c>
       <c r="D6" s="8">
         <v>1</v>
       </c>
-      <c r="E6" s="13">
-        <v>1158</v>
+      <c r="E6" s="31">
+        <v>1.1579999999999999</v>
       </c>
       <c r="F6" s="8">
         <v>9</v>
@@ -787,7 +914,7 @@
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
-      <c r="E7" s="14"/>
+      <c r="E7" s="32"/>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
     </row>
@@ -796,16 +923,16 @@
         <v>11</v>
       </c>
       <c r="B8" s="6">
-        <v>7.798</v>
+        <v>7798</v>
       </c>
       <c r="C8" s="6">
-        <v>7.835</v>
+        <v>7835</v>
       </c>
       <c r="D8" s="6">
         <v>1</v>
       </c>
-      <c r="E8" s="13">
-        <v>1005</v>
+      <c r="E8" s="31">
+        <v>1.0049999999999999</v>
       </c>
       <c r="F8" s="6">
         <v>2</v>
@@ -819,22 +946,22 @@
         <v>12</v>
       </c>
       <c r="B9" s="6">
-        <v>9.5739999999999998</v>
+        <v>9574</v>
       </c>
       <c r="C9" s="6">
-        <v>9.2070000000000007</v>
+        <v>9207</v>
       </c>
       <c r="D9" s="6">
         <v>1</v>
       </c>
-      <c r="E9" s="13">
-        <v>1361</v>
+      <c r="E9" s="31">
+        <v>1.361</v>
       </c>
       <c r="F9" s="6">
         <v>90</v>
       </c>
       <c r="G9" s="6">
-        <v>1.6519999999999999</v>
+        <v>1652</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -842,22 +969,22 @@
         <v>13</v>
       </c>
       <c r="B10" s="6">
-        <v>10.318</v>
+        <v>10318</v>
       </c>
       <c r="C10" s="6">
-        <v>9.3149999999999995</v>
+        <v>9315</v>
       </c>
       <c r="D10" s="6">
         <v>1</v>
       </c>
-      <c r="E10" s="13">
-        <v>1377</v>
+      <c r="E10" s="31">
+        <v>1.377</v>
       </c>
       <c r="F10" s="6">
         <v>91</v>
       </c>
       <c r="G10" s="6">
-        <v>1.895</v>
+        <v>1895</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
@@ -867,7 +994,7 @@
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
-      <c r="E11" s="14"/>
+      <c r="E11" s="32"/>
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
     </row>
@@ -876,22 +1003,22 @@
         <v>11</v>
       </c>
       <c r="B12" s="6">
-        <v>21.652999999999999</v>
+        <v>21653</v>
       </c>
       <c r="C12" s="6">
-        <v>30.643999999999998</v>
+        <v>30644</v>
       </c>
       <c r="D12" s="6">
         <v>1</v>
       </c>
-      <c r="E12" s="13">
-        <v>1416</v>
+      <c r="E12" s="31">
+        <v>1.4159999999999999</v>
       </c>
       <c r="F12" s="6">
         <v>4</v>
       </c>
       <c r="G12" s="6">
-        <v>8.9329999999999998</v>
+        <v>8933</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
@@ -899,22 +1026,22 @@
         <v>12</v>
       </c>
       <c r="B13" s="6">
-        <v>21.652999999999999</v>
+        <v>21653</v>
       </c>
       <c r="C13" s="6">
-        <v>31.734999999999999</v>
+        <v>31735</v>
       </c>
       <c r="D13" s="6">
         <v>2</v>
       </c>
-      <c r="E13" s="13">
-        <v>2070</v>
+      <c r="E13" s="31">
+        <v>2.0699999999999998</v>
       </c>
       <c r="F13" s="6">
         <v>294</v>
       </c>
       <c r="G13" s="6">
-        <v>11.314</v>
+        <v>11314</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
@@ -922,22 +1049,22 @@
         <v>13</v>
       </c>
       <c r="B14" s="6">
-        <v>21.652999999999999</v>
+        <v>21653</v>
       </c>
       <c r="C14" s="6">
-        <v>31.736000000000001</v>
+        <v>31736</v>
       </c>
       <c r="D14" s="6">
         <v>2</v>
       </c>
-      <c r="E14" s="13">
-        <v>2133</v>
+      <c r="E14" s="31">
+        <v>2.133</v>
       </c>
       <c r="F14" s="6">
         <v>294</v>
       </c>
       <c r="G14" s="6">
-        <v>12.269</v>
+        <v>12269</v>
       </c>
     </row>
   </sheetData>
@@ -954,238 +1081,245 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="28.1796875" customWidth="1"/>
+    <col min="2" max="2" width="11.26953125" style="25" customWidth="1"/>
+    <col min="3" max="3" width="11.453125" style="25" customWidth="1"/>
+    <col min="4" max="4" width="9.1796875" style="25"/>
+    <col min="5" max="5" width="9.1796875" style="20"/>
+    <col min="6" max="6" width="9.1796875" style="25"/>
+    <col min="7" max="7" width="11.54296875" style="25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="3"/>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="15" t="s">
+      <c r="A1" s="14"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="4"/>
+      <c r="G1" s="27"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="8">
-        <v>2.9889999999999999</v>
-      </c>
-      <c r="C2" s="8">
-        <v>2.9990000000000001</v>
-      </c>
-      <c r="D2" s="8">
+      <c r="B2" s="22">
+        <v>2989</v>
+      </c>
+      <c r="C2" s="22">
+        <v>2999</v>
+      </c>
+      <c r="D2" s="22">
         <v>1</v>
       </c>
-      <c r="E2" s="13">
-        <v>1006</v>
-      </c>
-      <c r="F2" s="8">
+      <c r="E2" s="18">
+        <v>1.006</v>
+      </c>
+      <c r="F2" s="22">
         <v>2</v>
       </c>
-      <c r="G2" s="8">
+      <c r="G2" s="28">
         <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="8">
-        <v>3.621</v>
-      </c>
-      <c r="C3" s="8">
-        <v>3.15</v>
-      </c>
-      <c r="D3" s="8">
+      <c r="B3" s="22">
+        <v>3621</v>
+      </c>
+      <c r="C3" s="22">
+        <v>3150</v>
+      </c>
+      <c r="D3" s="22">
         <v>1</v>
       </c>
-      <c r="E3" s="13">
-        <v>1145</v>
-      </c>
-      <c r="F3" s="8">
+      <c r="E3" s="18">
+        <v>1.145</v>
+      </c>
+      <c r="F3" s="22">
         <v>9</v>
       </c>
-      <c r="G3" s="8">
+      <c r="G3" s="28">
         <v>378</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="9">
-        <v>3.944</v>
-      </c>
-      <c r="C4" s="8">
-        <v>3.1520000000000001</v>
-      </c>
-      <c r="D4" s="8">
+      <c r="B4" s="23">
+        <v>3944</v>
+      </c>
+      <c r="C4" s="22">
+        <v>3152</v>
+      </c>
+      <c r="D4" s="22">
         <v>1</v>
       </c>
-      <c r="E4" s="13">
-        <v>1158</v>
-      </c>
-      <c r="F4" s="8">
+      <c r="E4" s="18">
+        <v>1.1579999999999999</v>
+      </c>
+      <c r="F4" s="22">
         <v>9</v>
       </c>
-      <c r="G4" s="8">
+      <c r="G4" s="28">
         <v>444</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="8">
-        <v>7.798</v>
-      </c>
-      <c r="C5" s="8">
-        <v>7.835</v>
-      </c>
-      <c r="D5" s="8">
+      <c r="B5" s="22">
+        <v>7798</v>
+      </c>
+      <c r="C5" s="22">
+        <v>7835</v>
+      </c>
+      <c r="D5" s="22">
         <v>1</v>
       </c>
-      <c r="E5" s="13">
-        <v>1005</v>
-      </c>
-      <c r="F5" s="8">
+      <c r="E5" s="18">
+        <v>1.0049999999999999</v>
+      </c>
+      <c r="F5" s="22">
         <v>2</v>
       </c>
-      <c r="G5" s="8">
+      <c r="G5" s="28">
         <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="8">
-        <v>9.5739999999999998</v>
-      </c>
-      <c r="C6" s="8">
-        <v>9.2070000000000007</v>
-      </c>
-      <c r="D6" s="8">
+      <c r="B6" s="22">
+        <v>9574</v>
+      </c>
+      <c r="C6" s="22">
+        <v>9207</v>
+      </c>
+      <c r="D6" s="22">
         <v>1</v>
       </c>
-      <c r="E6" s="13">
-        <v>1361</v>
-      </c>
-      <c r="F6" s="8">
+      <c r="E6" s="18">
+        <v>1.361</v>
+      </c>
+      <c r="F6" s="22">
         <v>90</v>
       </c>
-      <c r="G6" s="8">
-        <v>1.6519999999999999</v>
+      <c r="G6" s="28">
+        <v>1652</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="8">
-        <v>10.318</v>
-      </c>
-      <c r="C7" s="8">
-        <v>9.3149999999999995</v>
-      </c>
-      <c r="D7" s="8">
+      <c r="B7" s="22">
+        <v>10318</v>
+      </c>
+      <c r="C7" s="22">
+        <v>9315</v>
+      </c>
+      <c r="D7" s="22">
         <v>1</v>
       </c>
-      <c r="E7" s="13">
-        <v>1377</v>
-      </c>
-      <c r="F7" s="8">
+      <c r="E7" s="18">
+        <v>1.377</v>
+      </c>
+      <c r="F7" s="22">
         <v>91</v>
       </c>
-      <c r="G7" s="8">
-        <v>1.895</v>
+      <c r="G7" s="28">
+        <v>1895</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="8">
-        <v>21.652999999999999</v>
-      </c>
-      <c r="C8" s="8">
-        <v>30.643999999999998</v>
-      </c>
-      <c r="D8" s="8">
+      <c r="B8" s="22">
+        <v>21653</v>
+      </c>
+      <c r="C8" s="22">
+        <v>30644</v>
+      </c>
+      <c r="D8" s="22">
         <v>1</v>
       </c>
-      <c r="E8" s="13">
-        <v>1416</v>
-      </c>
-      <c r="F8" s="8">
+      <c r="E8" s="18">
+        <v>1.4159999999999999</v>
+      </c>
+      <c r="F8" s="22">
         <v>4</v>
       </c>
-      <c r="G8" s="8">
-        <v>8.9329999999999998</v>
+      <c r="G8" s="28">
+        <v>8933</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="8">
-        <v>21.652999999999999</v>
-      </c>
-      <c r="C9" s="8">
-        <v>31.734999999999999</v>
-      </c>
-      <c r="D9" s="8">
+      <c r="B9" s="22">
+        <v>21653</v>
+      </c>
+      <c r="C9" s="22">
+        <v>31735</v>
+      </c>
+      <c r="D9" s="22">
         <v>2</v>
       </c>
-      <c r="E9" s="13">
-        <v>2070</v>
-      </c>
-      <c r="F9" s="8">
+      <c r="E9" s="18">
+        <v>2.0699999999999998</v>
+      </c>
+      <c r="F9" s="22">
         <v>294</v>
       </c>
-      <c r="G9" s="8">
-        <v>11.314</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10" s="11" t="s">
+      <c r="G9" s="28">
+        <v>11314</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="8">
-        <v>21.652999999999999</v>
-      </c>
-      <c r="C10" s="8">
-        <v>31.736000000000001</v>
-      </c>
-      <c r="D10" s="8">
+      <c r="B10" s="24">
+        <v>21653</v>
+      </c>
+      <c r="C10" s="24">
+        <v>31736</v>
+      </c>
+      <c r="D10" s="24">
         <v>2</v>
       </c>
-      <c r="E10" s="13">
-        <v>2133</v>
-      </c>
-      <c r="F10" s="8">
+      <c r="E10" s="19">
+        <v>2.133</v>
+      </c>
+      <c r="F10" s="24">
         <v>294</v>
       </c>
-      <c r="G10" s="8">
-        <v>12.269</v>
+      <c r="G10" s="29">
+        <v>12269</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1413,18 +1547,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1447,26 +1581,26 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A9E6229F-9180-4EE6-8B1E-95613B60BA1D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="c13751bf-2e61-4f3e-8aba-d7ae2540d3c1"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="993ccfa7-7427-47b6-8e45-6e99719fb274"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BCB37E79-9967-44F3-946B-282A0312798E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A9E6229F-9180-4EE6-8B1E-95613B60BA1D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="993ccfa7-7427-47b6-8e45-6e99719fb274"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="c13751bf-2e61-4f3e-8aba-d7ae2540d3c1"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>